<commit_message>
new template nervosity 2
</commit_message>
<xml_diff>
--- a/templates/template_metric_nervosity.xlsx
+++ b/templates/template_metric_nervosity.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiss\Nextcloud\Manuscrit-relectures\Applications\Analyse_resultats\Template_Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiss\Nextcloud\SC_DSS_SIMU\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B72579F-0DD8-4257-A888-DCEC7757D4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F6302C-8693-4E09-9D74-405291668024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1" sheetId="1" r:id="rId1"/>
     <sheet name="P2" sheetId="2" r:id="rId2"/>
-    <sheet name="P3" sheetId="3" r:id="rId3"/>
-    <sheet name="P4" sheetId="4" r:id="rId4"/>
+    <sheet name="P4" sheetId="4" r:id="rId3"/>
+    <sheet name="P3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="34">
   <si>
     <t>Nervosité moyenne par période</t>
   </si>
@@ -133,13 +133,19 @@
   </si>
   <si>
     <t>France</t>
+  </si>
+  <si>
+    <t>Unvailability</t>
+  </si>
+  <si>
+    <t>Totale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +157,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -224,11 +238,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +524,602 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:AQ31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26">
+        <v>9</v>
+      </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
+      <c r="L26">
+        <v>11</v>
+      </c>
+      <c r="M26">
+        <v>12</v>
+      </c>
+      <c r="N26">
+        <v>13</v>
+      </c>
+      <c r="O26">
+        <v>14</v>
+      </c>
+      <c r="P26">
+        <v>15</v>
+      </c>
+      <c r="Q26">
+        <v>16</v>
+      </c>
+      <c r="R26">
+        <v>17</v>
+      </c>
+      <c r="S26">
+        <v>18</v>
+      </c>
+      <c r="T26">
+        <v>19</v>
+      </c>
+      <c r="U26">
+        <v>20</v>
+      </c>
+      <c r="V26">
+        <v>21</v>
+      </c>
+      <c r="W26">
+        <v>22</v>
+      </c>
+      <c r="X26">
+        <v>23</v>
+      </c>
+      <c r="Y26">
+        <v>24</v>
+      </c>
+      <c r="Z26">
+        <v>25</v>
+      </c>
+      <c r="AA26">
+        <v>26</v>
+      </c>
+      <c r="AB26">
+        <v>27</v>
+      </c>
+      <c r="AC26">
+        <v>28</v>
+      </c>
+      <c r="AD26">
+        <v>29</v>
+      </c>
+      <c r="AE26">
+        <v>30</v>
+      </c>
+      <c r="AF26">
+        <v>31</v>
+      </c>
+      <c r="AG26">
+        <v>32</v>
+      </c>
+      <c r="AH26">
+        <v>33</v>
+      </c>
+      <c r="AI26">
+        <v>34</v>
+      </c>
+      <c r="AJ26">
+        <v>35</v>
+      </c>
+      <c r="AK26">
+        <v>36</v>
+      </c>
+      <c r="AL26">
+        <v>37</v>
+      </c>
+      <c r="AM26">
+        <v>38</v>
+      </c>
+      <c r="AN26">
+        <v>39</v>
+      </c>
+      <c r="AO26">
+        <v>40</v>
+      </c>
+      <c r="AP26">
+        <v>41</v>
+      </c>
+      <c r="AQ26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BD56A0-5FFF-4599-B6E4-9797FC666E56}">
+  <dimension ref="A1:AQ31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+      <selection activeCell="A25" sqref="A25:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,102 +1447,177 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="1" t="s">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26">
         <v>9</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="K26">
         <v>10</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="L26">
         <v>11</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="M26">
         <v>12</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="N26">
         <v>13</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="O26">
         <v>14</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="P26">
         <v>15</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="Q26">
         <v>16</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="R26">
         <v>17</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="S26">
         <v>18</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="T26">
         <v>19</v>
       </c>
-      <c r="N20" s="2" t="s">
+      <c r="U26">
         <v>20</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="V26">
         <v>21</v>
       </c>
-      <c r="P20" s="2" t="s">
+      <c r="W26">
         <v>22</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="X26">
         <v>23</v>
       </c>
-      <c r="R20" s="2" t="s">
+      <c r="Y26">
         <v>24</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="Z26">
         <v>25</v>
       </c>
-      <c r="T20" s="2" t="s">
+      <c r="AA26">
         <v>26</v>
       </c>
-      <c r="U20" s="2" t="s">
+      <c r="AB26">
         <v>27</v>
       </c>
-      <c r="V20" s="3" t="s">
+      <c r="AC26">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="AD26">
+        <v>29</v>
+      </c>
+      <c r="AE26">
+        <v>30</v>
+      </c>
+      <c r="AF26">
+        <v>31</v>
+      </c>
+      <c r="AG26">
+        <v>32</v>
+      </c>
+      <c r="AH26">
+        <v>33</v>
+      </c>
+      <c r="AI26">
+        <v>34</v>
+      </c>
+      <c r="AJ26">
+        <v>35</v>
+      </c>
+      <c r="AK26">
+        <v>36</v>
+      </c>
+      <c r="AL26">
+        <v>37</v>
+      </c>
+      <c r="AM26">
+        <v>38</v>
+      </c>
+      <c r="AN26">
+        <v>39</v>
+      </c>
+      <c r="AO26">
+        <v>40</v>
+      </c>
+      <c r="AP26">
+        <v>41</v>
+      </c>
+      <c r="AQ26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>6</v>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -943,12 +1625,291 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BD56A0-5FFF-4599-B6E4-9797FC666E56}">
-  <dimension ref="A1:V19"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30103FFD-70AE-444C-A789-332A9838704E}">
+  <dimension ref="A1:AQ31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="22" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="43" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26">
+        <v>9</v>
+      </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
+      <c r="L26">
+        <v>11</v>
+      </c>
+      <c r="M26">
+        <v>12</v>
+      </c>
+      <c r="N26">
+        <v>13</v>
+      </c>
+      <c r="O26">
+        <v>14</v>
+      </c>
+      <c r="P26">
+        <v>15</v>
+      </c>
+      <c r="Q26">
+        <v>16</v>
+      </c>
+      <c r="R26">
+        <v>17</v>
+      </c>
+      <c r="S26">
+        <v>18</v>
+      </c>
+      <c r="T26">
+        <v>19</v>
+      </c>
+      <c r="U26">
+        <v>20</v>
+      </c>
+      <c r="V26">
+        <v>21</v>
+      </c>
+      <c r="W26">
+        <v>22</v>
+      </c>
+      <c r="X26">
+        <v>23</v>
+      </c>
+      <c r="Y26">
+        <v>24</v>
+      </c>
+      <c r="Z26">
+        <v>25</v>
+      </c>
+      <c r="AA26">
+        <v>26</v>
+      </c>
+      <c r="AB26">
+        <v>27</v>
+      </c>
+      <c r="AC26">
+        <v>28</v>
+      </c>
+      <c r="AD26">
+        <v>29</v>
+      </c>
+      <c r="AE26">
+        <v>30</v>
+      </c>
+      <c r="AF26">
+        <v>31</v>
+      </c>
+      <c r="AG26">
+        <v>32</v>
+      </c>
+      <c r="AH26">
+        <v>33</v>
+      </c>
+      <c r="AI26">
+        <v>34</v>
+      </c>
+      <c r="AJ26">
+        <v>35</v>
+      </c>
+      <c r="AK26">
+        <v>36</v>
+      </c>
+      <c r="AL26">
+        <v>37</v>
+      </c>
+      <c r="AM26">
+        <v>38</v>
+      </c>
+      <c r="AN26">
+        <v>39</v>
+      </c>
+      <c r="AO26">
+        <v>40</v>
+      </c>
+      <c r="AP26">
+        <v>41</v>
+      </c>
+      <c r="AQ26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB80B29-B20A-4FE4-B716-AD786ADE0DB4}">
+  <dimension ref="A1:AQ31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A25" sqref="A25:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,12 +2007,12 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1118,18 +2079,24 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -1198,368 +2165,6 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V16" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB80B29-B20A-4FE4-B716-AD786ADE0DB4}">
-  <dimension ref="A1:V15"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
@@ -1582,120 +2187,159 @@
         <v>6</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30103FFD-70AE-444C-A789-332A9838704E}">
-  <dimension ref="A1:V7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+      <c r="J26">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="K26">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="L26">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="M26">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="N26">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="O26">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="P26">
         <v>15</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="Q26">
         <v>16</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="R26">
         <v>17</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="S26">
         <v>18</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="T26">
         <v>19</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="U26">
         <v>20</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="V26">
         <v>21</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="W26">
         <v>22</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="X26">
         <v>23</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="Y26">
         <v>24</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="Z26">
         <v>25</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="AA26">
         <v>26</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="AB26">
         <v>27</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="AC26">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="AD26">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
+      <c r="AE26">
+        <v>30</v>
+      </c>
+      <c r="AF26">
+        <v>31</v>
+      </c>
+      <c r="AG26">
+        <v>32</v>
+      </c>
+      <c r="AH26">
+        <v>33</v>
+      </c>
+      <c r="AI26">
+        <v>34</v>
+      </c>
+      <c r="AJ26">
+        <v>35</v>
+      </c>
+      <c r="AK26">
+        <v>36</v>
+      </c>
+      <c r="AL26">
+        <v>37</v>
+      </c>
+      <c r="AM26">
+        <v>38</v>
+      </c>
+      <c r="AN26">
+        <v>39</v>
+      </c>
+      <c r="AO26">
+        <v>40</v>
+      </c>
+      <c r="AP26">
+        <v>41</v>
+      </c>
+      <c r="AQ26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modif 3 template nervosity
</commit_message>
<xml_diff>
--- a/templates/template_metric_nervosity.xlsx
+++ b/templates/template_metric_nervosity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stiss\Nextcloud\SC_DSS_SIMU\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F6302C-8693-4E09-9D74-405291668024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B295038-FE71-484C-8FA3-1948AFFB2515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="34">
   <si>
     <t>Nervosité moyenne par période</t>
   </si>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BD56A0-5FFF-4599-B6E4-9797FC666E56}">
-  <dimension ref="A1:AQ31"/>
+  <dimension ref="A1:AQ30"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD31"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1470,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>2</v>
       </c>
@@ -1607,16 +1607,11 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1627,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30103FFD-70AE-444C-A789-332A9838704E}">
-  <dimension ref="A1:AQ31"/>
+  <dimension ref="A1:AQ28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,21 +1879,6 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1906,10 +1886,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB80B29-B20A-4FE4-B716-AD786ADE0DB4}">
-  <dimension ref="A1:AQ31"/>
+  <dimension ref="A1:AQ29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,26 +2299,16 @@
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>